<commit_message>
results ND, AD, dAD
</commit_message>
<xml_diff>
--- a/Experimental data.xlsx
+++ b/Experimental data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20202379\Documents\GitHub\Algorithms-for-Model-Checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB85BF91-F7A0-4742-A6AD-719A408D5A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2F726-83AB-4143-A004-7A7AD30E94CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{119C8ED8-2447-C247-920A-6EBC15D5BD9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{119C8ED8-2447-C247-920A-6EBC15D5BD9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1207,10 +1207,10 @@
         <v>28</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1309,20 +1309,56 @@
       <c r="A16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>58</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>